<commit_message>
final tidy results and deletion
</commit_message>
<xml_diff>
--- a/Assignment/Data/Bank/bank-additional/Results tidy.xlsx
+++ b/Assignment/Data/Bank/bank-additional/Results tidy.xlsx
@@ -4,16 +4,15 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KNN" sheetId="8" r:id="rId1"/>
     <sheet name="DT" sheetId="9" r:id="rId2"/>
     <sheet name="RF" sheetId="10" r:id="rId3"/>
     <sheet name="NB" sheetId="11" r:id="rId4"/>
-    <sheet name="SVC" sheetId="12" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="20">
   <si>
     <t>nn=100</t>
   </si>
@@ -1531,8 +1530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{437C4C99-3C74-4132-B8AE-320AC7751DD9}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1869,7 +1868,7 @@
         <v>0.91</v>
       </c>
       <c r="H13" s="5">
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="I13" s="6">
         <v>0.62</v>
@@ -1901,10 +1900,10 @@
         <v>0.92</v>
       </c>
       <c r="H14" s="5">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="I14" s="6">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="J14" s="7">
         <v>0.9</v>
@@ -1959,7 +1958,8 @@
       <c r="H16" s="5"/>
       <c r="I16" s="6"/>
       <c r="J16" s="7">
-        <v>0.91</v>
+        <f>ROUND((H17+I18)/J19,2)</f>
+        <v>0.9</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1983,10 +1983,10 @@
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="5">
-        <v>10621</v>
+        <v>7660</v>
       </c>
       <c r="I17" s="6">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="J17" s="7">
         <v>8024</v>
@@ -2015,10 +2015,10 @@
         <v>12357</v>
       </c>
       <c r="H18" s="5">
-        <v>727</v>
+        <v>537</v>
       </c>
       <c r="I18" s="6">
-        <v>663</v>
+        <v>586</v>
       </c>
       <c r="J18" s="7">
         <v>1123</v>
@@ -2050,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C57C68-477D-406F-86F5-5E486C207B00}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2071,19 +2071,13 @@
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="E2" s="2"/>
       <c r="F2" s="3"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="3"/>
       <c r="J2" s="4"/>
     </row>
@@ -2097,120 +2091,72 @@
       <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5">
-        <v>0.93</v>
+        <v>0.95</v>
       </c>
       <c r="C4" s="6">
-        <v>0.64</v>
+        <v>0.49</v>
       </c>
       <c r="D4" s="7">
-        <v>0.89</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.93</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0.62</v>
-      </c>
-      <c r="G4" s="7">
-        <v>0.89</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0.92</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0.65</v>
-      </c>
-      <c r="J4" s="7">
-        <v>0.89</v>
-      </c>
+        <v>0.9</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="5">
-        <v>0.97</v>
+        <v>0.92</v>
       </c>
       <c r="C5" s="6">
-        <v>0.39</v>
+        <v>0.61</v>
       </c>
       <c r="D5" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.97</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0.41</v>
-      </c>
-      <c r="G5" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.97</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0.36</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0.91</v>
-      </c>
+        <v>0.54</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="5">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="C6" s="6">
-        <v>0.49</v>
+        <v>0.54</v>
       </c>
       <c r="D6" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0.47</v>
-      </c>
-      <c r="J6" s="7">
         <v>0.89</v>
       </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -2219,82 +2165,54 @@
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="7">
-        <v>0.91</v>
+        <v>0.88</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="7">
-        <v>0.91</v>
-      </c>
+      <c r="G7" s="7"/>
       <c r="H7" s="5"/>
       <c r="I7" s="6"/>
-      <c r="J7" s="7">
-        <v>0.91</v>
-      </c>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="5">
-        <v>10662</v>
+        <v>10081</v>
       </c>
       <c r="C8" s="6">
-        <v>305</v>
+        <v>886</v>
       </c>
       <c r="D8" s="7">
         <v>10967</v>
       </c>
-      <c r="E8" s="5">
-        <v>10617</v>
-      </c>
-      <c r="F8" s="6">
-        <v>350</v>
-      </c>
-      <c r="G8" s="7">
-        <v>10967</v>
-      </c>
-      <c r="H8" s="5">
-        <v>10690</v>
-      </c>
-      <c r="I8" s="6">
-        <v>277</v>
-      </c>
-      <c r="J8" s="7">
-        <v>10967</v>
-      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="5">
+        <v>546</v>
+      </c>
+      <c r="C9" s="6">
         <v>844</v>
-      </c>
-      <c r="C9" s="6">
-        <v>546</v>
       </c>
       <c r="D9" s="7">
         <v>1390</v>
       </c>
-      <c r="E9" s="5">
-        <v>815</v>
-      </c>
-      <c r="F9" s="6">
-        <v>575</v>
-      </c>
-      <c r="G9" s="7">
-        <v>1390</v>
-      </c>
-      <c r="H9" s="5">
-        <v>883</v>
-      </c>
-      <c r="I9" s="6">
-        <v>507</v>
-      </c>
-      <c r="J9" s="7">
-        <v>1390</v>
-      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="8"/>
@@ -2304,33 +2222,23 @@
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="10">
-        <v>12357</v>
-      </c>
+      <c r="G10" s="10"/>
       <c r="H10" s="8"/>
       <c r="I10" s="9"/>
-      <c r="J10" s="10">
-        <v>12357</v>
-      </c>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B11" s="2"/>
       <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="H11" s="2"/>
       <c r="I11" s="3" t="s">
         <v>10</v>
       </c>
@@ -2373,28 +2281,28 @@
         <v>0.94</v>
       </c>
       <c r="C13" s="6">
-        <v>0.63</v>
+        <v>0.42</v>
       </c>
       <c r="D13" s="7">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="E13" s="5">
         <v>0.94</v>
       </c>
       <c r="F13" s="6">
-        <v>0.63</v>
+        <v>0.36</v>
       </c>
       <c r="G13" s="7">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="H13" s="5">
-        <v>0.92</v>
+        <v>0.94</v>
       </c>
       <c r="I13" s="6">
-        <v>0.66</v>
+        <v>0.5</v>
       </c>
       <c r="J13" s="7">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -2402,31 +2310,31 @@
         <v>5</v>
       </c>
       <c r="B14" s="5">
-        <v>0.96</v>
+        <v>0.91</v>
       </c>
       <c r="C14" s="6">
-        <v>0.48</v>
+        <v>0.52</v>
       </c>
       <c r="D14" s="7">
-        <v>0.91</v>
+        <v>0.87</v>
       </c>
       <c r="E14" s="5">
-        <v>0.96</v>
+        <v>0.87</v>
       </c>
       <c r="F14" s="6">
-        <v>0.48</v>
+        <v>0.59</v>
       </c>
       <c r="G14" s="7">
-        <v>0.91</v>
+        <v>0.84</v>
       </c>
       <c r="H14" s="5">
-        <v>0.97</v>
+        <v>0.92</v>
       </c>
       <c r="I14" s="6">
-        <v>0.4</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J14" s="7">
-        <v>0.9</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -2434,31 +2342,31 @@
         <v>6</v>
       </c>
       <c r="B15" s="5">
-        <v>0.95</v>
+        <v>0.92</v>
       </c>
       <c r="C15" s="6">
-        <v>0.55000000000000004</v>
+        <v>0.47</v>
       </c>
       <c r="D15" s="7">
-        <v>0.9</v>
+        <v>0.87</v>
       </c>
       <c r="E15" s="5">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="F15" s="6">
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
       <c r="G15" s="7">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="H15" s="5">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="I15" s="6">
-        <v>0.5</v>
+        <v>0.53</v>
       </c>
       <c r="J15" s="7">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -2468,17 +2376,17 @@
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
       <c r="D16" s="7">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="6"/>
       <c r="G16" s="7">
-        <v>0.91</v>
+        <v>0.84</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="6"/>
       <c r="J16" s="7">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2486,26 +2394,26 @@
         <v>1</v>
       </c>
       <c r="B17" s="5">
-        <v>10576</v>
+        <v>10574</v>
       </c>
       <c r="C17" s="6">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D17" s="7">
         <v>10967</v>
       </c>
       <c r="E17" s="5">
-        <v>10576</v>
+        <v>9503</v>
       </c>
       <c r="F17" s="6">
-        <v>391</v>
+        <v>1464</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="5">
-        <v>7796</v>
+        <v>7383</v>
       </c>
       <c r="I17" s="6">
-        <v>228</v>
+        <v>641</v>
       </c>
       <c r="J17" s="7">
         <v>8024</v>
@@ -2516,28 +2424,28 @@
         <v>2</v>
       </c>
       <c r="B18" s="5">
-        <v>721</v>
+        <v>655</v>
       </c>
       <c r="C18" s="6">
-        <v>669</v>
+        <v>735</v>
       </c>
       <c r="D18" s="7">
         <v>1390</v>
       </c>
       <c r="E18" s="5">
-        <v>721</v>
+        <v>563</v>
       </c>
       <c r="F18" s="6">
-        <v>669</v>
+        <v>827</v>
       </c>
       <c r="G18" s="7">
         <v>12357</v>
       </c>
       <c r="H18" s="5">
-        <v>671</v>
+        <v>486</v>
       </c>
       <c r="I18" s="6">
-        <v>452</v>
+        <v>637</v>
       </c>
       <c r="J18" s="7">
         <v>1123</v>
@@ -2563,523 +2471,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F83B211-CBD0-4E6D-B750-6BF216272E4E}">
-  <dimension ref="A1:M19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5">
-        <v>0.93</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0.64</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0.89</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.93</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0.62</v>
-      </c>
-      <c r="G4" s="7">
-        <v>0.89</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0.92</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0.65</v>
-      </c>
-      <c r="J4" s="7">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0.97</v>
-      </c>
-      <c r="C5" s="6">
-        <v>0.39</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.97</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0.41</v>
-      </c>
-      <c r="G5" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.97</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0.36</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0.49</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0.47</v>
-      </c>
-      <c r="J6" s="7">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="5">
-        <v>10662</v>
-      </c>
-      <c r="C8" s="6">
-        <v>305</v>
-      </c>
-      <c r="D8" s="7">
-        <v>10967</v>
-      </c>
-      <c r="E8" s="5">
-        <v>10617</v>
-      </c>
-      <c r="F8" s="6">
-        <v>350</v>
-      </c>
-      <c r="G8" s="7">
-        <v>10967</v>
-      </c>
-      <c r="H8" s="5">
-        <v>10690</v>
-      </c>
-      <c r="I8" s="6">
-        <v>277</v>
-      </c>
-      <c r="J8" s="7">
-        <v>10967</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="5">
-        <v>844</v>
-      </c>
-      <c r="C9" s="6">
-        <v>546</v>
-      </c>
-      <c r="D9" s="7">
-        <v>1390</v>
-      </c>
-      <c r="E9" s="5">
-        <v>815</v>
-      </c>
-      <c r="F9" s="6">
-        <v>575</v>
-      </c>
-      <c r="G9" s="7">
-        <v>1390</v>
-      </c>
-      <c r="H9" s="5">
-        <v>883</v>
-      </c>
-      <c r="I9" s="6">
-        <v>507</v>
-      </c>
-      <c r="J9" s="7">
-        <v>1390</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10">
-        <v>12357</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10">
-        <v>12357</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10">
-        <v>12357</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="5">
-        <v>0.94</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0.63</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.94</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0.63</v>
-      </c>
-      <c r="G13" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.92</v>
-      </c>
-      <c r="I13" s="6">
-        <v>0.66</v>
-      </c>
-      <c r="J13" s="7">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="5">
-        <v>0.96</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0.48</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0.96</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0.48</v>
-      </c>
-      <c r="G14" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="H14" s="5">
-        <v>0.97</v>
-      </c>
-      <c r="I14" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="J14" s="7">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="E15" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G15" s="7">
-        <v>0.9</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="I15" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="J15" s="7">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="7">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="5">
-        <v>10576</v>
-      </c>
-      <c r="C17" s="6">
-        <v>391</v>
-      </c>
-      <c r="D17" s="7">
-        <v>10967</v>
-      </c>
-      <c r="E17" s="5">
-        <v>10576</v>
-      </c>
-      <c r="F17" s="6">
-        <v>391</v>
-      </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="5">
-        <v>7796</v>
-      </c>
-      <c r="I17" s="6">
-        <v>228</v>
-      </c>
-      <c r="J17" s="7">
-        <v>8024</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="5">
-        <v>721</v>
-      </c>
-      <c r="C18" s="6">
-        <v>669</v>
-      </c>
-      <c r="D18" s="7">
-        <v>1390</v>
-      </c>
-      <c r="E18" s="5">
-        <v>721</v>
-      </c>
-      <c r="F18" s="6">
-        <v>669</v>
-      </c>
-      <c r="G18" s="7">
-        <v>12357</v>
-      </c>
-      <c r="H18" s="5">
-        <v>671</v>
-      </c>
-      <c r="I18" s="6">
-        <v>452</v>
-      </c>
-      <c r="J18" s="7">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10">
-        <v>12357</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="10">
-        <v>12357</v>
-      </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="10">
-        <v>9147</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>